<commit_message>
Updated to remove reference to MPU-6050 and also to note that OMRON 2-position dip switch is sold out and backordered until June on most sites.
</commit_message>
<xml_diff>
--- a/resources/CharliesAlienWhoopF4BrushedPartsList.xlsx
+++ b/resources/CharliesAlienWhoopF4BrushedPartsList.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\charlies\Documents\Copter\AlienWeeF4\WhoopWii\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\charlies\Documents\eagle\CharliesAlienWhoopF4\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="153">
   <si>
     <t>Part</t>
   </si>
@@ -293,9 +293,6 @@
     <t>Invensense</t>
   </si>
   <si>
-    <t>MPU-6500</t>
-  </si>
-  <si>
     <t>U2</t>
   </si>
   <si>
@@ -480,6 +477,12 @@
   </si>
   <si>
     <t>Sidemount USB connector</t>
+  </si>
+  <si>
+    <t>MPU-9250</t>
+  </si>
+  <si>
+    <t>SOLDOUT</t>
   </si>
 </sst>
 </file>
@@ -560,12 +563,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -582,7 +591,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
@@ -600,6 +609,9 @@
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="44" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -1077,7 +1089,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="175" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:XFD7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1112,36 +1126,36 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>97</v>
       </c>
       <c r="F2" s="2">
         <v>0.41</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -1164,7 +1178,7 @@
         <v>0.24</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -1227,27 +1241,30 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:8" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C7" s="1" t="s">
+      <c r="B7" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="C7" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="D7" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="18">
         <v>2.17</v>
       </c>
-      <c r="H7" s="3" t="s">
-        <v>148</v>
+      <c r="G7" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="H7" s="19" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -1270,7 +1287,7 @@
         <v>0.21</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -1293,7 +1310,7 @@
         <v>0.21</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -1336,7 +1353,7 @@
         <v>0.11</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
@@ -1441,19 +1458,19 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>100</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>20</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F17" s="2">
         <v>0.44</v>
@@ -1479,7 +1496,7 @@
         <v>0.46</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
@@ -1606,7 +1623,7 @@
       </c>
       <c r="G24" s="6"/>
       <c r="H24" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="25" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -1630,7 +1647,7 @@
       </c>
       <c r="G25" s="8"/>
       <c r="H25" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="26" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -1780,7 +1797,7 @@
       </c>
       <c r="G32" s="6"/>
       <c r="H32" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="33" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -1825,7 +1842,7 @@
       </c>
       <c r="G34" s="8"/>
       <c r="H34" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="35" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -1863,14 +1880,14 @@
         <v>88</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>89</v>
+        <v>151</v>
       </c>
       <c r="F36" s="8"/>
       <c r="G36" s="8">
         <v>10.64</v>
       </c>
       <c r="H36" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
@@ -1884,13 +1901,13 @@
         <v>45</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
@@ -1898,7 +1915,7 @@
         <v>46</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>47</v>
@@ -1913,7 +1930,7 @@
         <v>0.23</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
@@ -1936,104 +1953,104 @@
         <v>10.58</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="C40" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="D40" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="E40" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>94</v>
       </c>
       <c r="F40" s="2">
         <v>2.25</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="C41" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="D41" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="D41" s="1" t="s">
-        <v>130</v>
-      </c>
       <c r="E41" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G41" s="2">
         <v>2</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C42" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B42" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="C42" s="1" t="s">
+      <c r="D42" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="E42" s="13" t="s">
         <v>135</v>
-      </c>
-      <c r="E42" s="13" t="s">
-        <v>136</v>
       </c>
       <c r="G42" s="14">
         <v>6.5</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B43" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="C43" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D43" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="E43" s="13" t="s">
         <v>143</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="E43" s="13" t="s">
-        <v>144</v>
       </c>
       <c r="G43" s="2">
         <v>7.8</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="45" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="15" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F45" s="16">
         <f>SUM(F2:F43)</f>
@@ -2046,7 +2063,7 @@
     </row>
     <row r="46" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="15" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F46" s="16"/>
       <c r="G46" s="16">
@@ -2054,32 +2071,32 @@
         <v>48.382999999999996</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E48" s="7"/>
       <c r="H48" s="11"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G52" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="53" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -2087,10 +2104,10 @@
         <v>80</v>
       </c>
       <c r="B53" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C53" s="3" t="s">
         <v>121</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>122</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>15</v>
@@ -2103,7 +2120,7 @@
         <v>0.66</v>
       </c>
       <c r="H53" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="54" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Substituted the sealed version of the OMRON dip switch since the unsealed are backordered until June. Maybe they're trying to reduce inventory?
</commit_message>
<xml_diff>
--- a/resources/CharliesAlienWhoopF4BrushedPartsList.xlsx
+++ b/resources/CharliesAlienWhoopF4BrushedPartsList.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="148">
   <si>
     <t>Part</t>
   </si>
@@ -155,15 +155,6 @@
     <t>C13</t>
   </si>
   <si>
-    <t>JP1</t>
-  </si>
-  <si>
-    <t>3-PAD</t>
-  </si>
-  <si>
-    <t>3 way Solder Pad</t>
-  </si>
-  <si>
     <t>L1</t>
   </si>
   <si>
@@ -278,18 +269,12 @@
     <t>OMRON</t>
   </si>
   <si>
-    <t>A6H-2101</t>
-  </si>
-  <si>
     <t>U1</t>
   </si>
   <si>
     <t>MPU9250</t>
   </si>
   <si>
-    <t>MPU-6500/9250</t>
-  </si>
-  <si>
     <t>Invensense</t>
   </si>
   <si>
@@ -362,9 +347,6 @@
     <t>Mouser 10 @.044c</t>
   </si>
   <si>
-    <t>PPM or Satellite RX</t>
-  </si>
-  <si>
     <t>N/A</t>
   </si>
   <si>
@@ -467,9 +449,6 @@
     <t>Grand total</t>
   </si>
   <si>
-    <t>Feel free to not buy this and manually jumper</t>
-  </si>
-  <si>
     <t>IMPORTANT to order BLUE and only BLUE</t>
   </si>
   <si>
@@ -482,7 +461,13 @@
     <t>MPU-9250</t>
   </si>
   <si>
-    <t>SOLDOUT</t>
+    <t>A6H-2102</t>
+  </si>
+  <si>
+    <t>Substituted for A6H-2101 (backordered)</t>
+  </si>
+  <si>
+    <t>9-Axis Motion Sensor</t>
   </si>
 </sst>
 </file>
@@ -563,18 +548,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -591,7 +570,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
@@ -609,9 +588,6 @@
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="44" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -803,8 +779,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H52" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="A1:H52"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H51" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="A1:H51"/>
   <sortState ref="A2:H44">
     <sortCondition ref="E2:E44"/>
     <sortCondition ref="B2:B44"/>
@@ -1087,11 +1063,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H55"/>
+  <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="175" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1126,50 +1100,50 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="F2" s="2">
         <v>0.41</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>5</v>
@@ -1178,21 +1152,21 @@
         <v>0.24</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>5</v>
@@ -1203,16 +1177,16 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>5</v>
@@ -1223,16 +1197,16 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>5</v>
@@ -1241,30 +1215,27 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="B7" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>122</v>
-      </c>
-      <c r="D7" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="E7" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="F7" s="18">
-        <v>2.17</v>
-      </c>
-      <c r="G7" s="18" t="s">
-        <v>152</v>
-      </c>
-      <c r="H7" s="19" t="s">
-        <v>147</v>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="F7" s="2">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -1287,7 +1258,7 @@
         <v>0.21</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -1310,12 +1281,12 @@
         <v>0.21</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>7</v>
@@ -1335,42 +1306,42 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>74</v>
       </c>
       <c r="F11" s="2">
         <v>0.11</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>74</v>
       </c>
       <c r="F12" s="2">
         <v>0.11</v>
@@ -1378,19 +1349,19 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>74</v>
       </c>
       <c r="F13" s="2">
         <v>0.11</v>
@@ -1398,19 +1369,19 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>74</v>
       </c>
       <c r="F14" s="2">
         <v>0.11</v>
@@ -1418,19 +1389,19 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>74</v>
       </c>
       <c r="F15" s="2">
         <v>0.11</v>
@@ -1438,19 +1409,19 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>74</v>
       </c>
       <c r="F16" s="2">
         <v>0.11</v>
@@ -1458,19 +1429,19 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>20</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F17" s="2">
         <v>0.44</v>
@@ -1478,42 +1449,42 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="E18" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F18" s="2">
         <v>0.46</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F19" s="2">
         <v>0.46</v>
@@ -1521,19 +1492,19 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F20" s="2">
         <v>0.46</v>
@@ -1541,19 +1512,19 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F21" s="2">
         <v>0.46</v>
@@ -1623,7 +1594,7 @@
       </c>
       <c r="G24" s="6"/>
       <c r="H24" s="7" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="25" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -1647,7 +1618,7 @@
       </c>
       <c r="G25" s="8"/>
       <c r="H25" s="5" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="26" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -1797,24 +1768,24 @@
       </c>
       <c r="G32" s="6"/>
       <c r="H32" s="7" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="33" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D33" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B33" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>67</v>
-      </c>
       <c r="E33" s="5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F33" s="8">
         <v>0.38</v>
@@ -1842,7 +1813,7 @@
       </c>
       <c r="G34" s="8"/>
       <c r="H34" s="5" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="35" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -1868,26 +1839,26 @@
     </row>
     <row r="36" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>87</v>
+        <v>147</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="F36" s="8"/>
       <c r="G36" s="8">
         <v>10.64</v>
       </c>
       <c r="H36" s="5" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
@@ -1895,88 +1866,91 @@
         <v>43</v>
       </c>
       <c r="B37" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C37" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="D37" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E37" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D37" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>113</v>
+      <c r="F37" s="2">
+        <v>0.23</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>124</v>
+        <v>54</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F38" s="2">
-        <v>0.23</v>
+        <v>54</v>
+      </c>
+      <c r="G38" s="2">
+        <v>10.58</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>55</v>
+        <v>84</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>57</v>
+        <v>85</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>57</v>
+        <v>86</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>56</v>
+        <v>87</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="G39" s="2">
-        <v>10.58</v>
+        <v>88</v>
+      </c>
+      <c r="F39" s="2">
+        <v>2.25</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>89</v>
+        <v>120</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>90</v>
+        <v>121</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>91</v>
+        <v>122</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>92</v>
+        <v>123</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F40" s="2">
-        <v>2.25</v>
+        <v>107</v>
+      </c>
+      <c r="G40" s="2">
+        <v>2</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
@@ -1984,175 +1958,152 @@
         <v>126</v>
       </c>
       <c r="B41" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C41" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="D41" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="E41" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="E41" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="G41" s="2">
-        <v>2</v>
+      <c r="G41" s="14">
+        <v>6.5</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E42" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="G42" s="14">
-        <v>6.5</v>
+        <v>137</v>
+      </c>
+      <c r="G42" s="2">
+        <v>7.8</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A43" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="15" t="s">
         <v>139</v>
       </c>
-      <c r="B43" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="E43" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="G43" s="2">
-        <v>7.8</v>
-      </c>
-      <c r="H43" s="1" t="s">
-        <v>144</v>
+      <c r="F44" s="16">
+        <f>SUM(F2:F42)</f>
+        <v>11.243000000000002</v>
+      </c>
+      <c r="G44" s="16">
+        <f>SUM(G2:G42)</f>
+        <v>37.519999999999996</v>
       </c>
     </row>
     <row r="45" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="15" t="s">
-        <v>145</v>
-      </c>
-      <c r="F45" s="16">
-        <f>SUM(F2:F43)</f>
-        <v>10.863000000000001</v>
-      </c>
+        <v>140</v>
+      </c>
+      <c r="F45" s="16"/>
       <c r="G45" s="16">
-        <f>SUM(G2:G43)</f>
-        <v>37.519999999999996</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="F46" s="16"/>
-      <c r="G46" s="16">
-        <f>F45+G45</f>
-        <v>48.382999999999996</v>
-      </c>
-      <c r="H46" s="3" t="s">
-        <v>149</v>
-      </c>
+        <f>F44+G44</f>
+        <v>48.762999999999998</v>
+      </c>
+      <c r="H45" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E47" s="7"/>
+      <c r="H47" s="11"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="E48" s="7"/>
-      <c r="H48" s="11"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A50" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A51" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="G51" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="G52" s="4" t="s">
-        <v>102</v>
+        <v>77</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F52" s="4"/>
+      <c r="G52" s="4">
+        <v>0.66</v>
+      </c>
+      <c r="H52" s="3" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="53" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
-        <v>80</v>
+        <v>12</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>120</v>
+        <v>13</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>121</v>
+        <v>14</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>81</v>
+        <v>16</v>
       </c>
       <c r="F53" s="4"/>
       <c r="G53" s="4">
-        <v>0.66</v>
-      </c>
-      <c r="H53" s="3" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D54" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E54" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F54" s="4"/>
-      <c r="G54" s="4">
         <v>0.17</v>
       </c>
     </row>
-    <row r="55" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="F55" s="10"/>
-      <c r="G55" s="10"/>
-      <c r="H55" s="12"/>
+    <row r="54" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F54" s="10"/>
+      <c r="G54" s="10"/>
+      <c r="H54" s="12"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E42" r:id="rId1" display="http://docs.oshpark.com/services/two-layer-hhdc/"/>
-    <hyperlink ref="E43" r:id="rId2"/>
+    <hyperlink ref="E41" r:id="rId1" display="http://docs.oshpark.com/services/two-layer-hhdc/"/>
+    <hyperlink ref="E42" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>

</xml_diff>